<commit_message>
more forms to add and 3 new libraries
</commit_message>
<xml_diff>
--- a/PRIMERAS TABLAS.xlsx.xlsx
+++ b/PRIMERAS TABLAS.xlsx.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="313">
   <si>
     <t>PACIENTES</t>
   </si>
@@ -955,6 +955,9 @@
   </si>
   <si>
     <t>active_principle</t>
+  </si>
+  <si>
+    <t>COMPAÑÍA</t>
   </si>
 </sst>
 </file>
@@ -1059,20 +1062,20 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1357,20 +1360,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="E248" sqref="E248"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="26" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="26" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11"/>
@@ -1601,8 +1605,8 @@
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>52</v>
+      <c r="A26" s="10" t="s">
+        <v>312</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="1" t="s">
@@ -1714,7 +1718,7 @@
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B39" s="11"/>
@@ -1783,7 +1787,7 @@
       <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="10" t="s">
         <v>78</v>
       </c>
       <c r="B47" s="11"/>
@@ -1851,7 +1855,7 @@
       <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
+      <c r="A55" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B55" s="11"/>
@@ -1901,7 +1905,7 @@
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="10" t="s">
         <v>96</v>
       </c>
       <c r="B61" s="11"/>
@@ -1993,7 +1997,7 @@
       <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
+      <c r="A71" s="12" t="s">
         <v>111</v>
       </c>
       <c r="B71" s="11"/>
@@ -2129,7 +2133,7 @@
       <c r="C86" s="1"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="s">
+      <c r="A87" s="12" t="s">
         <v>128</v>
       </c>
       <c r="B87" s="11"/>
@@ -2171,7 +2175,7 @@
       <c r="C91" s="1"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="13" t="s">
+      <c r="A92" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B92" s="11"/>
@@ -2203,7 +2207,7 @@
       <c r="C95" s="1"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="13" t="s">
+      <c r="A96" s="12" t="s">
         <v>132</v>
       </c>
       <c r="B96" s="11"/>
@@ -2244,7 +2248,7 @@
       <c r="C100" s="1"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="13" t="s">
+      <c r="A101" s="12" t="s">
         <v>137</v>
       </c>
       <c r="B101" s="11"/>
@@ -2299,7 +2303,7 @@
       <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="10" t="s">
+      <c r="A108" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B108" s="11"/>
@@ -2369,7 +2373,7 @@
       <c r="C115" s="1"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="13" t="s">
+      <c r="A116" s="12" t="s">
         <v>147</v>
       </c>
       <c r="B116" s="11"/>
@@ -2485,7 +2489,7 @@
       <c r="C128" s="1"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="10" t="s">
+      <c r="A129" s="13" t="s">
         <v>162</v>
       </c>
       <c r="B129" s="11"/>
@@ -2632,7 +2636,7 @@
       <c r="C145" s="1"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="12" t="s">
+      <c r="A146" s="15" t="s">
         <v>182</v>
       </c>
       <c r="B146" s="11"/>
@@ -2714,7 +2718,7 @@
       <c r="C155" s="1"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="12" t="s">
+      <c r="A156" s="15" t="s">
         <v>194</v>
       </c>
       <c r="B156" s="11"/>
@@ -2764,7 +2768,7 @@
       <c r="C161" s="1"/>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="12" t="s">
+      <c r="A162" s="15" t="s">
         <v>200</v>
       </c>
       <c r="B162" s="11"/>
@@ -2811,7 +2815,7 @@
       <c r="C166" s="1"/>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="12" t="s">
+      <c r="A167" s="15" t="s">
         <v>205</v>
       </c>
       <c r="B167" s="11"/>
@@ -2852,7 +2856,7 @@
       <c r="C171" s="1"/>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="12" t="s">
+      <c r="A172" s="15" t="s">
         <v>209</v>
       </c>
       <c r="B172" s="11"/>
@@ -2884,7 +2888,7 @@
       <c r="C175" s="1"/>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" s="12" t="s">
+      <c r="A176" s="15" t="s">
         <v>211</v>
       </c>
       <c r="B176" s="11"/>
@@ -2921,7 +2925,7 @@
       <c r="C179" s="1"/>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="12" t="s">
+      <c r="A180" s="15" t="s">
         <v>214</v>
       </c>
       <c r="B180" s="11"/>
@@ -2967,7 +2971,7 @@
       <c r="C185" s="1"/>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" s="12" t="s">
+      <c r="A186" s="15" t="s">
         <v>218</v>
       </c>
       <c r="B186" s="11"/>
@@ -3060,7 +3064,7 @@
       <c r="C196" s="1"/>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="12" t="s">
+      <c r="A197" s="15" t="s">
         <v>234</v>
       </c>
       <c r="B197" s="11"/>
@@ -3092,7 +3096,7 @@
       <c r="C200" s="1"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="12" t="s">
+      <c r="A201" s="15" t="s">
         <v>236</v>
       </c>
       <c r="B201" s="11"/>
@@ -3133,7 +3137,7 @@
       <c r="C205" s="1"/>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206" s="12" t="s">
+      <c r="A206" s="15" t="s">
         <v>241</v>
       </c>
       <c r="B206" s="11"/>
@@ -3165,7 +3169,7 @@
       <c r="C209" s="1"/>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="12" t="s">
+      <c r="A210" s="15" t="s">
         <v>243</v>
       </c>
       <c r="B210" s="11"/>
@@ -3197,7 +3201,7 @@
       <c r="C213" s="1"/>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="10" t="s">
+      <c r="A214" s="13" t="s">
         <v>245</v>
       </c>
       <c r="B214" s="11"/>
@@ -3409,7 +3413,7 @@
       <c r="C237" s="1"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" s="12" t="s">
+      <c r="A238" s="15" t="s">
         <v>284</v>
       </c>
       <c r="B238" s="11"/>
@@ -3441,7 +3445,7 @@
       <c r="C241" s="1"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" s="12" t="s">
+      <c r="A242" s="15" t="s">
         <v>286</v>
       </c>
       <c r="B242" s="11"/>
@@ -3482,7 +3486,7 @@
       <c r="C246" s="1"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A247" s="12" t="s">
+      <c r="A247" s="15" t="s">
         <v>289</v>
       </c>
       <c r="B247" s="11"/>
@@ -3514,7 +3518,7 @@
       <c r="C250" s="1"/>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A251" s="10" t="s">
+      <c r="A251" s="13" t="s">
         <v>291</v>
       </c>
       <c r="B251" s="11"/>
@@ -7325,6 +7329,27 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A251:B251"/>
+    <mergeCell ref="A247:B247"/>
+    <mergeCell ref="A242:B242"/>
+    <mergeCell ref="A238:B238"/>
+    <mergeCell ref="A186:B186"/>
+    <mergeCell ref="A197:B197"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="A206:B206"/>
+    <mergeCell ref="A210:B210"/>
+    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="A172:B172"/>
+    <mergeCell ref="A162:B162"/>
+    <mergeCell ref="A176:B176"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A156:B156"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A101:B101"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A116:B116"/>
@@ -7335,27 +7360,6 @@
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A108:B108"/>
     <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A146:B146"/>
-    <mergeCell ref="A156:B156"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A167:B167"/>
-    <mergeCell ref="A172:B172"/>
-    <mergeCell ref="A162:B162"/>
-    <mergeCell ref="A176:B176"/>
-    <mergeCell ref="A180:B180"/>
-    <mergeCell ref="A251:B251"/>
-    <mergeCell ref="A247:B247"/>
-    <mergeCell ref="A242:B242"/>
-    <mergeCell ref="A238:B238"/>
-    <mergeCell ref="A186:B186"/>
-    <mergeCell ref="A197:B197"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="A206:B206"/>
-    <mergeCell ref="A210:B210"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
change to the main route
</commit_message>
<xml_diff>
--- a/PRIMERAS TABLAS.xlsx.xlsx
+++ b/PRIMERAS TABLAS.xlsx.xlsx
@@ -964,7 +964,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1005,12 +1005,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1061,7 +1055,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1077,13 +1071,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1094,7 +1084,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1377,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B223" sqref="B223"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A251" sqref="A251:B251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1391,10 +1381,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1622,10 +1612,10 @@
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="14" t="s">
         <v>311</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="1" t="s">
         <v>53</v>
       </c>
@@ -1735,10 +1725,10 @@
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="17"/>
+      <c r="B39" s="15"/>
       <c r="C39" s="1" t="s">
         <v>72</v>
       </c>
@@ -1804,10 +1794,10 @@
       <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B47" s="17"/>
+      <c r="B47" s="15"/>
       <c r="C47" s="1" t="s">
         <v>79</v>
       </c>
@@ -1872,10 +1862,10 @@
       <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="17"/>
+      <c r="B55" s="15"/>
       <c r="C55" s="1" t="s">
         <v>92</v>
       </c>
@@ -1922,10 +1912,10 @@
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B61" s="17"/>
+      <c r="B61" s="15"/>
       <c r="C61" s="1" t="s">
         <v>97</v>
       </c>
@@ -2014,10 +2004,10 @@
       <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+      <c r="A71" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B71" s="14"/>
+      <c r="B71" s="12"/>
       <c r="C71" s="1" t="s">
         <v>112</v>
       </c>
@@ -2150,10 +2140,10 @@
       <c r="C86" s="1"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="15" t="s">
+      <c r="A87" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B87" s="14"/>
+      <c r="B87" s="12"/>
       <c r="C87" s="1" t="s">
         <v>129</v>
       </c>
@@ -2192,10 +2182,10 @@
       <c r="C91" s="1"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="15" t="s">
+      <c r="A92" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B92" s="14"/>
+      <c r="B92" s="12"/>
       <c r="C92" s="1" t="s">
         <v>130</v>
       </c>
@@ -2224,10 +2214,10 @@
       <c r="C95" s="1"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="15" t="s">
+      <c r="A96" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="B96" s="14"/>
+      <c r="B96" s="12"/>
       <c r="C96" s="1" t="s">
         <v>133</v>
       </c>
@@ -2265,10 +2255,10 @@
       <c r="C100" s="1"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="15" t="s">
+      <c r="A101" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B101" s="14"/>
+      <c r="B101" s="12"/>
       <c r="C101" s="9" t="s">
         <v>138</v>
       </c>
@@ -2320,10 +2310,10 @@
       <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="13" t="s">
+      <c r="A108" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B108" s="14"/>
+      <c r="B108" s="12"/>
       <c r="C108" s="1" t="s">
         <v>141</v>
       </c>
@@ -2390,10 +2380,10 @@
       <c r="C115" s="1"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="15" t="s">
+      <c r="A116" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="B116" s="14"/>
+      <c r="B116" s="12"/>
       <c r="C116" s="1" t="s">
         <v>148</v>
       </c>
@@ -2506,10 +2496,10 @@
       <c r="C128" s="1"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="13" t="s">
+      <c r="A129" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B129" s="14"/>
+      <c r="B129" s="12"/>
       <c r="C129" s="1" t="s">
         <v>163</v>
       </c>
@@ -2653,10 +2643,10 @@
       <c r="C145" s="1"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="13" t="s">
+      <c r="A146" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B146" s="14"/>
+      <c r="B146" s="12"/>
       <c r="C146" s="1" t="s">
         <v>183</v>
       </c>
@@ -2735,10 +2725,10 @@
       <c r="C155" s="1"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" s="13" t="s">
+      <c r="A156" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="B156" s="14"/>
+      <c r="B156" s="12"/>
       <c r="C156" s="1" t="s">
         <v>195</v>
       </c>
@@ -2785,10 +2775,10 @@
       <c r="C161" s="1"/>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="13" t="s">
+      <c r="A162" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B162" s="14"/>
+      <c r="B162" s="12"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1" t="s">
         <v>201</v>
@@ -2832,10 +2822,10 @@
       <c r="C166" s="1"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="13" t="s">
+      <c r="A167" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="B167" s="14"/>
+      <c r="B167" s="12"/>
       <c r="C167" s="1" t="s">
         <v>206</v>
       </c>
@@ -2873,10 +2863,10 @@
       <c r="C171" s="1"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="13" t="s">
+      <c r="A172" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B172" s="14"/>
+      <c r="B172" s="12"/>
       <c r="C172" s="10" t="s">
         <v>210</v>
       </c>
@@ -2905,10 +2895,10 @@
       <c r="C175" s="1"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="13" t="s">
+      <c r="A176" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="B176" s="14"/>
+      <c r="B176" s="12"/>
       <c r="C176" s="1" t="s">
         <v>212</v>
       </c>
@@ -2939,10 +2929,10 @@
       <c r="C179" s="1"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" s="13" t="s">
+      <c r="A180" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="B180" s="14"/>
+      <c r="B180" s="12"/>
       <c r="C180" s="1" t="s">
         <v>215</v>
       </c>
@@ -2985,10 +2975,10 @@
       <c r="C185" s="1"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" s="13" t="s">
+      <c r="A186" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="B186" s="14"/>
+      <c r="B186" s="12"/>
       <c r="C186" s="1" t="s">
         <v>219</v>
       </c>
@@ -3078,10 +3068,10 @@
       <c r="C196" s="1"/>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A197" s="13" t="s">
+      <c r="A197" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="B197" s="14"/>
+      <c r="B197" s="12"/>
       <c r="C197" s="1" t="s">
         <v>235</v>
       </c>
@@ -3110,10 +3100,10 @@
       <c r="C200" s="1"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A201" s="13" t="s">
+      <c r="A201" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="B201" s="14"/>
+      <c r="B201" s="12"/>
       <c r="C201" s="1" t="s">
         <v>237</v>
       </c>
@@ -3151,10 +3141,10 @@
       <c r="C205" s="1"/>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A206" s="13" t="s">
+      <c r="A206" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="B206" s="14"/>
+      <c r="B206" s="12"/>
       <c r="C206" s="1" t="s">
         <v>242</v>
       </c>
@@ -3183,11 +3173,11 @@
       <c r="C209" s="1"/>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A210" s="13" t="s">
+      <c r="A210" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="B210" s="14"/>
-      <c r="C210" s="18" t="s">
+      <c r="B210" s="12"/>
+      <c r="C210" s="16" t="s">
         <v>244</v>
       </c>
     </row>
@@ -3215,10 +3205,10 @@
       <c r="C213" s="1"/>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A214" s="13" t="s">
+      <c r="A214" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="B214" s="14"/>
+      <c r="B214" s="12"/>
       <c r="C214" s="1" t="s">
         <v>246</v>
       </c>
@@ -3427,10 +3417,10 @@
       <c r="C237" s="1"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" s="13" t="s">
+      <c r="A238" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="B238" s="14"/>
+      <c r="B238" s="12"/>
       <c r="C238" s="1" t="s">
         <v>285</v>
       </c>
@@ -3459,10 +3449,10 @@
       <c r="C241" s="1"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A242" s="13" t="s">
+      <c r="A242" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="B242" s="14"/>
+      <c r="B242" s="12"/>
       <c r="C242" s="1" t="s">
         <v>287</v>
       </c>

</xml_diff>